<commit_message>
Fixed BOM file. Added missing 4 channel level shifter
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin Beym\Documents\PlatformIO\Projects\EnclosureController_ESP32\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0172715C-FD6A-45F2-AB1A-5C27D68F7ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1CC082-7ACB-4989-B5F1-7E731DD32767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AE960CD-5628-4DFF-862D-CAA157149A78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>This file includes all components needed to assemble the pcb</t>
   </si>
@@ -237,6 +237,24 @@
   </si>
   <si>
     <t>12v Led strip</t>
+  </si>
+  <si>
+    <t>can be less</t>
+  </si>
+  <si>
+    <t>can be none</t>
+  </si>
+  <si>
+    <t>can be less/none</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>Bi-Direktional 4 Channel Level Shifter</t>
+  </si>
+  <si>
+    <t>https://www.banggood.com/Logic-Level-Converter-Bi-Directional-IIC-4-Way-Level-Conversion-Module-p-938774.html?rmmds=detail-left-hotproducts__8&amp;cur_warehouse=CN</t>
   </si>
 </sst>
 </file>
@@ -329,12 +347,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -348,11 +360,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3219AD82-1188-4513-A6B1-85A1AAA7734F}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,34 +707,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,7 +745,7 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
@@ -735,7 +753,7 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -753,74 +771,74 @@
       <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="10"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -829,105 +847,105 @@
       <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
@@ -937,7 +955,7 @@
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
@@ -945,7 +963,7 @@
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
@@ -953,10 +971,13 @@
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -965,61 +986,76 @@
       <c r="D22" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="5">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5">
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="5">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="5">
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="5">
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1028,13 +1064,16 @@
       <c r="D27" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1043,39 +1082,63 @@
       <c r="D28" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="10"/>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A19:E21"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E3"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="E13:E18"/>
     <mergeCell ref="A4:E5"/>
-    <mergeCell ref="A19:E21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{C0117CED-FF00-41C3-B32F-F465DA6BC1DF}"/>
@@ -1087,8 +1150,9 @@
     <hyperlink ref="E22" r:id="rId7" xr:uid="{F42B22C8-FA57-49B4-9FC3-AA7FD22ED662}"/>
     <hyperlink ref="E23" r:id="rId8" xr:uid="{64AF41C0-B9A8-4596-B071-9D647F664F35}"/>
     <hyperlink ref="E25" r:id="rId9" xr:uid="{8CE3A461-BC2E-4C34-9FFF-8676FE046C72}"/>
+    <hyperlink ref="E30" r:id="rId10" xr:uid="{C0800E57-6F98-43BA-91B8-47AA18F5D366}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>